<commit_message>
Flight IDs rework for fighters. ATO and mission update. Resolve #1
</commit_message>
<xml_diff>
--- a/doc/TR_AD_doc_ATO.xlsx
+++ b/doc/TR_AD_doc_ATO.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\couby\Desktop\Saved Games\DCS.openbeta\Missions\TR_AD_Caucasus_One\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88205560-E9A6-4149-92C8-1E17477E2918}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562E7FDB-67C5-4DAD-B0AB-91F86FEEE6D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4395" yWindow="-14895" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="ATO" sheetId="1" r:id="rId1"/>
+    <sheet name="Affectation indicatifs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
-  <si>
-    <t>Indicatif</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="85">
   <si>
     <t>Task</t>
   </si>
@@ -60,88 +58,229 @@
     <t>CAP Alpha</t>
   </si>
   <si>
-    <t>Colt1</t>
-  </si>
-  <si>
     <t>M-2000C</t>
   </si>
   <si>
-    <t>Colt3</t>
-  </si>
-  <si>
     <t>F-14B</t>
   </si>
   <si>
-    <t>Enfield1</t>
-  </si>
-  <si>
-    <t>Enfield2</t>
-  </si>
-  <si>
     <t>SWEEP Alpha</t>
   </si>
   <si>
-    <t>Enfield3</t>
-  </si>
-  <si>
-    <t>Enfield4</t>
-  </si>
-  <si>
-    <t>Enfield5</t>
-  </si>
-  <si>
-    <t>Enfield6</t>
-  </si>
-  <si>
-    <t>Enfield7</t>
-  </si>
-  <si>
-    <t>Enfield8</t>
-  </si>
-  <si>
     <t>SWEEP Bravo</t>
   </si>
   <si>
-    <t>Flanker9</t>
-  </si>
-  <si>
     <t>CAP Bravo</t>
   </si>
   <si>
     <t>Tbilissi</t>
   </si>
   <si>
-    <t>Fury9</t>
-  </si>
-  <si>
-    <t>Springfield1</t>
-  </si>
-  <si>
-    <t>Springfield2</t>
-  </si>
-  <si>
-    <t>Springfield3</t>
-  </si>
-  <si>
-    <t>Uzi1</t>
-  </si>
-  <si>
     <t>CAP Charlie</t>
   </si>
   <si>
-    <t>Uzi2</t>
-  </si>
-  <si>
-    <t>Uzi3</t>
-  </si>
-  <si>
-    <t>Weasel9</t>
-  </si>
-  <si>
     <t>AAR</t>
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Indicatif2</t>
+  </si>
+  <si>
+    <t>Enfield</t>
+  </si>
+  <si>
+    <t>Springfield</t>
+  </si>
+  <si>
+    <t>Uzi</t>
+  </si>
+  <si>
+    <t>Colt</t>
+  </si>
+  <si>
+    <t>Dodge</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Chevy</t>
+  </si>
+  <si>
+    <t>Pontiac</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>Sweep</t>
+  </si>
+  <si>
+    <t>Chalice</t>
+  </si>
+  <si>
+    <t>Cowboy</t>
+  </si>
+  <si>
+    <t>Viper</t>
+  </si>
+  <si>
+    <t>Lobo</t>
+  </si>
+  <si>
+    <t>Gypsy</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>Sting</t>
+  </si>
+  <si>
+    <t>Sentry</t>
+  </si>
+  <si>
+    <t>Weasel</t>
+  </si>
+  <si>
+    <t>Serpent</t>
+  </si>
+  <si>
+    <t>Fury</t>
+  </si>
+  <si>
+    <t>Falcon</t>
+  </si>
+  <si>
+    <t>Cobra</t>
+  </si>
+  <si>
+    <t>Camel</t>
+  </si>
+  <si>
+    <t>Bulldog</t>
+  </si>
+  <si>
+    <t>Ghost</t>
+  </si>
+  <si>
+    <t>Hornet</t>
+  </si>
+  <si>
+    <t>Mustang</t>
+  </si>
+  <si>
+    <t>Gator</t>
+  </si>
+  <si>
+    <t>Voodoo</t>
+  </si>
+  <si>
+    <t>Panther</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Mig</t>
+  </si>
+  <si>
+    <t>Flanker</t>
+  </si>
+  <si>
+    <t>Saint</t>
+  </si>
+  <si>
+    <t>Darkstar</t>
+  </si>
+  <si>
+    <t>Fazer</t>
+  </si>
+  <si>
+    <t>Cylon</t>
+  </si>
+  <si>
+    <t>Rambo</t>
+  </si>
+  <si>
+    <t>Raider</t>
+  </si>
+  <si>
+    <t>Evil</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Snake</t>
+  </si>
+  <si>
+    <t>Savage</t>
+  </si>
+  <si>
+    <t>Blue4</t>
+  </si>
+  <si>
+    <t>Bulldog2</t>
+  </si>
+  <si>
+    <t>Bulldog1</t>
+  </si>
+  <si>
+    <t>Bulldog4</t>
+  </si>
+  <si>
+    <t>Camel4</t>
+  </si>
+  <si>
+    <t>Camel1</t>
+  </si>
+  <si>
+    <t>Camel2</t>
+  </si>
+  <si>
+    <t>Chalice1</t>
+  </si>
+  <si>
+    <t>Chalice2</t>
+  </si>
+  <si>
+    <t>Chevy1</t>
+  </si>
+  <si>
+    <t>Chevy2</t>
+  </si>
+  <si>
+    <t>Cobra1</t>
+  </si>
+  <si>
+    <t>Cobra2</t>
+  </si>
+  <si>
+    <t>Cylon2</t>
+  </si>
+  <si>
+    <t>Darkstar2</t>
+  </si>
+  <si>
+    <t>Cowboy2</t>
+  </si>
+  <si>
+    <t>Evil3</t>
+  </si>
+  <si>
+    <t>Falcon3</t>
+  </si>
+  <si>
+    <t>Fazer3</t>
   </si>
 </sst>
 </file>
@@ -505,7 +644,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,331 +652,737 @@
     <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="4" width="4.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" customWidth="1"/>
+    <col min="11" max="12" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>27</v>
+        <v>4</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>9</v>
+      <c r="D18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E22">
+    <sortCondition ref="A2"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75A8B75-A170-47F5-B28E-E43EA035D692}">
+  <dimension ref="A1:D44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A44">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ATO completion and format improvement. Resolve #2
</commit_message>
<xml_diff>
--- a/doc/TR_AD_doc_ATO.xlsx
+++ b/doc/TR_AD_doc_ATO.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\couby\Desktop\Saved Games\DCS.openbeta\Missions\TR_AD_Caucasus_One\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562E7FDB-67C5-4DAD-B0AB-91F86FEEE6D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCF945A-9AD1-4306-ABD1-199FFF9F81EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4395" yWindow="-14895" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ATO" sheetId="1" r:id="rId1"/>
-    <sheet name="Affectation indicatifs" sheetId="2" r:id="rId2"/>
+    <sheet name="Blue ATO" sheetId="1" r:id="rId1"/>
+    <sheet name="IDs logic" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="96">
   <si>
     <t>Task</t>
   </si>
@@ -85,9 +85,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Indicatif2</t>
-  </si>
-  <si>
     <t>Enfield</t>
   </si>
   <si>
@@ -281,6 +278,42 @@
   </si>
   <si>
     <t>Fazer3</t>
+  </si>
+  <si>
+    <t>Texaco1</t>
+  </si>
+  <si>
+    <t>KC-135MPRS</t>
+  </si>
+  <si>
+    <t>Texaco2</t>
+  </si>
+  <si>
+    <t>KC-135</t>
+  </si>
+  <si>
+    <t>AAR ROZ Balpha</t>
+  </si>
+  <si>
+    <t>Batumi</t>
+  </si>
+  <si>
+    <t>Overlord1</t>
+  </si>
+  <si>
+    <t>E-3A</t>
+  </si>
+  <si>
+    <t>Group Callsign</t>
+  </si>
+  <si>
+    <t>GhostRider1</t>
+  </si>
+  <si>
+    <t>GhostRider2</t>
+  </si>
+  <si>
+    <t>CVN-74 Stennis</t>
   </si>
 </sst>
 </file>
@@ -311,7 +344,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -336,6 +369,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -349,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,6 +406,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,6 +426,1236 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>224790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Image 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EAB9AC1-5A7C-46D5-88B4-91303C11BCFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1046797" y="2765108"/>
+          <a:ext cx="203835" cy="240030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>224790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Image 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6845CAFE-46DE-4D1B-97C9-DAC9C60C35F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1046797" y="3041333"/>
+          <a:ext cx="203835" cy="240030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>224790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Image 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21AE27D8-DDA1-4970-BE2B-FAD64E47FE35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1046797" y="279083"/>
+          <a:ext cx="203835" cy="240030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>224790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Image 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDBBC835-7EF5-44B1-BC40-35F3554670D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1046797" y="555308"/>
+          <a:ext cx="203835" cy="240030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>224790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Image 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1601C104-CF31-4D92-A9BE-C7A447DD6E35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1046797" y="831533"/>
+          <a:ext cx="203835" cy="240030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>224790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Image 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95912FDB-4E9E-435E-A0FB-D77725C54E46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1046797" y="4422458"/>
+          <a:ext cx="203835" cy="240030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Image 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B19A2663-EDBF-4BB4-AE0E-581EB24E9D9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1046797" y="5256848"/>
+          <a:ext cx="207645" cy="243840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>251459</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Image 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{450ACD50-0C34-4120-B97B-7CC77D49BC38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="24291" t="20383" r="24253" b="22919"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1040054" y="6938086"/>
+          <a:ext cx="228751" cy="251459"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>251459</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Image 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{854E1EBA-7462-43D9-9A82-9BB5407A3638}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="24291" t="20383" r="24253" b="22919"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1040054" y="7214311"/>
+          <a:ext cx="228751" cy="251459"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>229552</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>212894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Image 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F9C037E-A061-43D7-975E-03E4486D4F6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1058936" y="1118479"/>
+          <a:ext cx="169079" cy="229552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>229552</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>212894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Image 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B01B1AE-9A59-4992-A0DA-EC3933C1A166}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1058936" y="1394704"/>
+          <a:ext cx="169079" cy="229552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>229552</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>212894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Image 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{568DE1F3-F8E3-43FC-ADF1-AF6D901E21E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1058936" y="1670929"/>
+          <a:ext cx="169079" cy="229552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>229552</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>212894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Image 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05D2B8ED-9897-45E6-885B-DAA2FD43EC56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1058936" y="3328279"/>
+          <a:ext cx="169079" cy="229552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>229552</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>212894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Image 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C251AEB-28CE-4DDF-BE8C-8F870A067D62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1058936" y="3604504"/>
+          <a:ext cx="169079" cy="229552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>229552</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>212894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Image 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C3D98B1-8F5B-4A9C-A0DB-C15DEFB5205A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1058936" y="4985629"/>
+          <a:ext cx="169079" cy="229552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>229552</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>212894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Image 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C2CEE4D-CF8A-43DA-B898-6842423B29BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1058936" y="6366754"/>
+          <a:ext cx="169079" cy="229552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>229552</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>212894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Image 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F6F2F61-1C60-40FD-B6D4-BA027BDC1EE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1058936" y="5538079"/>
+          <a:ext cx="169079" cy="229552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>268605</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>257097</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Image 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191EA59B-ED31-4DF8-91AB-FEB316D760A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1037312" y="1934488"/>
+          <a:ext cx="251382" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>268605</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>257097</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Image 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B83F6BD0-86A9-4773-9A02-05899C190120}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1037312" y="2210713"/>
+          <a:ext cx="251382" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>268605</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>257097</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Image 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A378F26A-AF21-4EF3-B0E7-FE0D9240FD43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1037312" y="2486938"/>
+          <a:ext cx="251382" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>268605</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>268527</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Image 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEFDEB6C-A937-4E3E-AAFD-A39446619AA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1039217" y="3877588"/>
+          <a:ext cx="247572" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>268605</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>268527</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Image 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFE447F4-6BD7-482D-B87F-E3C0B164297C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1039217" y="4153813"/>
+          <a:ext cx="247572" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>268605</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1827</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Image 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F490C2A7-AFDE-4294-8572-4227159C1A2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1037312" y="5818783"/>
+          <a:ext cx="251382" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>36195</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>268605</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>13257</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Image 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1AA08B8-B31C-4626-9DC6-1B66C4E895CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1038264" y="6103581"/>
+          <a:ext cx="249477" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>208597</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>249799</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Image 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30E30518-D6DF-41C9-948B-1D0442B5B2BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26826" t="24172" r="27551" b="26207"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1030007" y="7500583"/>
+          <a:ext cx="205984" cy="208597"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -641,348 +1921,452 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" customWidth="1"/>
-    <col min="11" max="12" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="4" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" customWidth="1"/>
+    <col min="12" max="13" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="F23" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="F24" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="6" t="s">
+    <row r="28" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
     <sortCondition ref="A2"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -998,13 +2382,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
@@ -1012,13 +2396,13 @@
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -1026,13 +2410,13 @@
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1040,13 +2424,13 @@
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -1054,13 +2438,13 @@
     </row>
     <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -1068,13 +2452,13 @@
     </row>
     <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1082,13 +2466,13 @@
     </row>
     <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -1096,13 +2480,13 @@
     </row>
     <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -1110,13 +2494,13 @@
     </row>
     <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1124,13 +2508,13 @@
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -1138,13 +2522,13 @@
     </row>
     <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -1152,13 +2536,13 @@
     </row>
     <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -1166,13 +2550,13 @@
     </row>
     <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -1180,13 +2564,13 @@
     </row>
     <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
@@ -1194,13 +2578,13 @@
     </row>
     <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -1208,13 +2592,13 @@
     </row>
     <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
@@ -1222,13 +2606,13 @@
     </row>
     <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
@@ -1236,13 +2620,13 @@
     </row>
     <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -1250,132 +2634,132 @@
     </row>
     <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test scoring et ATO update.
</commit_message>
<xml_diff>
--- a/doc/TR_AD_doc_ATO.xlsx
+++ b/doc/TR_AD_doc_ATO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\couby\Desktop\Saved Games\DCS.openbeta\Missions\TR_AD_Caucasus_One\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCF945A-9AD1-4306-ABD1-199FFF9F81EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC53DFA-9D4D-44D4-BF4A-9118477F233B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="-14895" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blue ATO" sheetId="1" r:id="rId1"/>
@@ -833,7 +833,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>251459</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>151</xdr:rowOff>
+      <xdr:rowOff>152</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1647,6 +1647,55 @@
         <a:xfrm rot="5400000">
           <a:off x="1030007" y="7500583"/>
           <a:ext cx="205984" cy="208597"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1905</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>247572</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Image 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4105D3C6-AF75-4928-A61D-7EB2803E3C72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1010642" y="4523383"/>
+          <a:ext cx="247572" cy="268605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1923,23 +1972,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="4.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" customWidth="1"/>
-    <col min="12" max="13" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="13" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>92</v>
       </c>
@@ -1957,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1972,7 +2021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1987,7 +2036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -2002,7 +2051,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -2017,7 +2066,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -2032,7 +2081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -2047,7 +2096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -2062,7 +2111,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -2077,7 +2126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2092,7 +2141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -2107,7 +2156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -2122,7 +2171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -2137,7 +2186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -2152,7 +2201,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -2167,7 +2216,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -2182,7 +2231,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -2200,7 +2249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -2218,7 +2267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -2236,7 +2285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>81</v>
       </c>
@@ -2251,7 +2300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -2266,7 +2315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -2281,7 +2330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -2296,7 +2345,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -2311,10 +2360,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
     </row>
-    <row r="26" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -2329,7 +2378,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -2344,7 +2393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -2378,9 +2427,9 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>50</v>
       </c>
@@ -2394,7 +2443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>43</v>
       </c>
@@ -2408,7 +2457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -2422,7 +2471,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -2436,7 +2485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -2450,7 +2499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -2464,7 +2513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -2478,7 +2527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -2492,7 +2541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>58</v>
       </c>
@@ -2506,7 +2555,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>56</v>
       </c>
@@ -2520,7 +2569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -2534,7 +2583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -2548,7 +2597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>61</v>
       </c>
@@ -2562,7 +2611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -2576,7 +2625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>57</v>
       </c>
@@ -2590,7 +2639,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
@@ -2604,7 +2653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -2618,7 +2667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
@@ -2632,132 +2681,132 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Add flights for airborne start. Resolve #13
</commit_message>
<xml_diff>
--- a/doc/TR_AD_doc_ATO.xlsx
+++ b/doc/TR_AD_doc_ATO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\couby\Saved Games\DCS.openbeta\Missions\735th_Training_AirDefense_Mission\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037A7C2B-11E6-4048-A3FA-65B9A5EBBE2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983275FC-255B-45A6-B2B8-0C86B64AA2B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="116">
   <si>
     <t>Task</t>
   </si>
@@ -358,13 +358,31 @@
   </si>
   <si>
     <t>Cobra3</t>
+  </si>
+  <si>
+    <t>Chalice4</t>
+  </si>
+  <si>
+    <t>Chevy4</t>
+  </si>
+  <si>
+    <t>Cobra4</t>
+  </si>
+  <si>
+    <t>Airborne start point</t>
+  </si>
+  <si>
+    <t>Thimphou</t>
+  </si>
+  <si>
+    <t>New York</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,8 +419,20 @@
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,8 +481,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -475,11 +511,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -519,15 +592,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,68 +632,68 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>20955</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>224790</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Image 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EAB9AC1-5A7C-46D5-88B4-91303C11BCFF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="1046797" y="2765108"/>
-          <a:ext cx="203835" cy="240030"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>224790</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Image 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EAB9AC1-5A7C-46D5-88B4-91303C11BCFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1046797" y="2765108"/>
+          <a:ext cx="203835" cy="240030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>224790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
         <xdr:cNvPr id="14" name="Image 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
@@ -647,72 +730,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>20955</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>224790</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Image 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21AE27D8-DDA1-4970-BE2B-FAD64E47FE35}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="1046797" y="279083"/>
-          <a:ext cx="203835" cy="240030"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>224790</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Image 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDBBC835-7EF5-44B1-BC40-35F3554670D1}"/>
+        <xdr:cNvPr id="15" name="Image 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21AE27D8-DDA1-4970-BE2B-FAD64E47FE35}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -733,7 +767,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1046797" y="555308"/>
+          <a:off x="1046797" y="279083"/>
           <a:ext cx="203835" cy="240030"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -745,19 +779,68 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>224790</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Image 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDBBC835-7EF5-44B1-BC40-35F3554670D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1046797" y="555308"/>
+          <a:ext cx="203835" cy="240030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>224790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
         <xdr:cNvPr id="17" name="Image 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
@@ -794,15 +877,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>224790</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -843,15 +926,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>238125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -892,15 +975,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>251459</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>151</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -941,15 +1024,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>251459</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>152</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -990,72 +1073,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>43815</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>229552</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>212894</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Image 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F9C037E-A061-43D7-975E-03E4486D4F6E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="1058936" y="1118479"/>
-          <a:ext cx="169079" cy="229552"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>229552</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>212894</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Image 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B01B1AE-9A59-4992-A0DA-EC3933C1A166}"/>
+        <xdr:cNvPr id="22" name="Image 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F9C037E-A061-43D7-975E-03E4486D4F6E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1076,7 +1110,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1058936" y="1394704"/>
+          <a:off x="1058936" y="1118479"/>
           <a:ext cx="169079" cy="229552"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1088,19 +1122,68 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>229552</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>212894</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Image 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B01B1AE-9A59-4992-A0DA-EC3933C1A166}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1058936" y="1394704"/>
+          <a:ext cx="169079" cy="229552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>229552</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>212894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
         <xdr:cNvPr id="24" name="Image 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
@@ -1137,15 +1220,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>229552</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>212894</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1186,15 +1269,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>229552</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>212894</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1235,15 +1318,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>229552</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>212894</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1284,15 +1367,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>229552</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>212894</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1333,15 +1416,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>229552</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>212894</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1382,72 +1465,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1905</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>257097</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Image 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191EA59B-ED31-4DF8-91AB-FEB316D760A2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="1037312" y="1934488"/>
-          <a:ext cx="251382" cy="268605"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1905</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>257097</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Image 30">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B83F6BD0-86A9-4773-9A02-05899C190120}"/>
+        <xdr:cNvPr id="30" name="Image 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191EA59B-ED31-4DF8-91AB-FEB316D760A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1468,7 +1502,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1037312" y="2210713"/>
+          <a:off x="1037312" y="1934488"/>
           <a:ext cx="251382" cy="268605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1480,19 +1514,68 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1905</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>257097</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Image 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B83F6BD0-86A9-4773-9A02-05899C190120}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1037312" y="2210713"/>
+          <a:ext cx="251382" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1905</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>257097</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
         <xdr:cNvPr id="32" name="Image 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
@@ -1529,15 +1612,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1905</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>1827</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1578,15 +1661,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1905</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>1827</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1627,15 +1710,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1905</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>1827</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1676,15 +1759,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>36195</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1905</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>13257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1725,15 +1808,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>208597</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>249799</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1774,15 +1857,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1905</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>247572</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1823,9 +1906,9 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="247650" cy="203835"/>
@@ -1867,9 +1950,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="229552" cy="169079"/>
@@ -1911,9 +1994,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="268605" cy="247572"/>
@@ -1955,18 +2038,150 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="268605" cy="247572"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Image 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18BCFDD6-C0D0-4938-A7C0-B19EEC0EB913}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1010642" y="4887238"/>
+          <a:ext cx="247572" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="247650" cy="203835"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Image 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97F40CFC-87AD-41B2-A2D4-130954C3D84B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1155382" y="3685223"/>
+          <a:ext cx="203835" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="229552" cy="169079"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Image 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86F66C2E-71E4-476E-A3F1-D70EBC92DEF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1163711" y="4766554"/>
+          <a:ext cx="169079" cy="229552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="268605" cy="247572"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="Image 41">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18BCFDD6-C0D0-4938-A7C0-B19EEC0EB913}"/>
+        <xdr:cNvPr id="45" name="Image 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5931C94-D2DF-423A-B541-15A4BBD6A336}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1987,7 +2202,95 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1010642" y="4887238"/>
+          <a:off x="1143992" y="5563513"/>
+          <a:ext cx="247572" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="268605" cy="247572"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Image 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04710A89-28DE-44F5-A32D-AC629897E534}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1143992" y="5563513"/>
+          <a:ext cx="247572" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="268605" cy="247572"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Image 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{950C022C-2A94-4763-A4D7-FB37AB7BD8AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1143992" y="5830213"/>
           <a:ext cx="247572" cy="268605"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3545,657 +3848,767 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="B1:J41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="13" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="4" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="14" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="2:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="I3" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="12" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="14" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H4" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="I4" s="26"/>
+    </row>
+    <row r="5" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="12" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="14" t="s">
+      <c r="F5" s="15"/>
+      <c r="G5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="H5" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="I5" s="26"/>
+    </row>
+    <row r="6" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="12" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="14" t="s">
+      <c r="F6" s="15"/>
+      <c r="G6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="H6" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="I6" s="26"/>
+    </row>
+    <row r="7" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="12" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="14" t="s">
+      <c r="F7" s="15"/>
+      <c r="G7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="H7" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="I7" s="26"/>
+    </row>
+    <row r="8" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="12" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="14" t="s">
+      <c r="F8" s="15"/>
+      <c r="G8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="H8" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="I8" s="26"/>
+    </row>
+    <row r="9" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="12" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="14" t="s">
+      <c r="F9" s="15"/>
+      <c r="G9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="H9" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="I9" s="26"/>
+    </row>
+    <row r="10" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="14" t="s">
+      <c r="F10" s="15"/>
+      <c r="G10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="H10" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="14" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="H11" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="I11" s="26"/>
+    </row>
+    <row r="12" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="12" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="14" t="s">
+      <c r="F12" s="15"/>
+      <c r="G12" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="H12" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="I12" s="26"/>
+    </row>
+    <row r="13" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="12" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="E13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="14" t="s">
+      <c r="F13" s="15"/>
+      <c r="G13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="H13" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="I13" s="26"/>
+    </row>
+    <row r="14" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="12" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="14" t="s">
+      <c r="F14" s="15"/>
+      <c r="G14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="H14" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="12" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="14" t="s">
+      <c r="F15" s="15"/>
+      <c r="G15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="H15" s="21" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="I15" s="26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="12" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="14" t="s">
+      <c r="F17" s="15"/>
+      <c r="G17" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="H17" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="I17" s="26"/>
+    </row>
+    <row r="18" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="12" t="s">
+      <c r="C18" s="13"/>
+      <c r="D18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="14" t="s">
+      <c r="F18" s="15"/>
+      <c r="G18" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="H18" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="I18" s="26"/>
+    </row>
+    <row r="19" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="12" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="14" t="s">
+      <c r="F19" s="15"/>
+      <c r="G19" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="H19" s="21" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="I19" s="26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="12" t="s">
+      <c r="C21" s="13"/>
+      <c r="D21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="E21" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="14" t="s">
+      <c r="F21" s="15"/>
+      <c r="G21" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="H21" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="12" t="s">
+      <c r="C22" s="13"/>
+      <c r="D22" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="E22" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="14" t="s">
+      <c r="F22" s="15"/>
+      <c r="G22" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="H22" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="12" t="s">
+      <c r="C23" s="13"/>
+      <c r="D23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="E23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="14" t="s">
+      <c r="F23" s="15"/>
+      <c r="G23" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="H23" s="21" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="I23" s="26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="12" t="s">
+      <c r="C25" s="13"/>
+      <c r="D25" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="E25" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="F25" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="G25" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="H25" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="I25" s="26"/>
+    </row>
+    <row r="26" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="12" t="s">
+      <c r="C26" s="13"/>
+      <c r="D26" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="E26" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="F26" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="G26" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="H26" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="I26" s="26"/>
+    </row>
+    <row r="27" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="12" t="s">
+      <c r="C27" s="13"/>
+      <c r="D27" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="E27" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="F27" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="G27" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="H27" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="I27" s="26"/>
+    </row>
+    <row r="28" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="12" t="s">
+      <c r="C28" s="13"/>
+      <c r="D28" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="E28" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="18" t="s">
+      <c r="F28" s="15"/>
+      <c r="G28" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="H28" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="I28" s="26"/>
+    </row>
+    <row r="29" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="12" t="s">
+      <c r="C29" s="13"/>
+      <c r="D29" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="E29" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="18" t="s">
+      <c r="F29" s="15"/>
+      <c r="G29" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="H29" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="I29" s="26"/>
+    </row>
+    <row r="30" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="12" t="s">
+      <c r="C30" s="13"/>
+      <c r="D30" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="E30" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="18" t="s">
+      <c r="F30" s="15"/>
+      <c r="G30" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="H30" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="I30" s="26"/>
+    </row>
+    <row r="31" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="12" t="s">
+      <c r="C31" s="13"/>
+      <c r="D31" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="E31" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="19" t="s">
+      <c r="F31" s="15"/>
+      <c r="G31" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="H31" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="I31" s="26"/>
+    </row>
+    <row r="32" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="12" t="s">
+      <c r="C32" s="13"/>
+      <c r="D32" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="E32" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="19" t="s">
+      <c r="F32" s="15"/>
+      <c r="G32" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="H32" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-    </row>
-    <row r="30" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="I32" s="26"/>
+    </row>
+    <row r="33" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="12"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="27"/>
+    </row>
+    <row r="34" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="12" t="s">
+      <c r="C34" s="13"/>
+      <c r="D34" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="E34" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="20" t="s">
+      <c r="F34" s="15"/>
+      <c r="G34" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="G30" s="16" t="s">
+      <c r="H34" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="I34" s="26"/>
+    </row>
+    <row r="35" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="12" t="s">
+      <c r="C35" s="13"/>
+      <c r="D35" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="E35" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="18" t="s">
+      <c r="F35" s="15"/>
+      <c r="G35" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="H35" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+      <c r="I35" s="26"/>
+    </row>
+    <row r="36" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="12" t="s">
+      <c r="C36" s="13"/>
+      <c r="D36" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="E36" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="18" t="s">
+      <c r="F36" s="15"/>
+      <c r="G36" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="16" t="s">
+      <c r="H36" s="16" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="35" spans="6:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="F35" s="8" t="s">
+      <c r="I36" s="26"/>
+    </row>
+    <row r="39" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G39" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="H39" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="I39" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="6:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="F36" s="8"/>
-      <c r="G36" s="9" t="s">
+    <row r="40" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G40" s="8"/>
+      <c r="H40" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="I40" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="6:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G37" s="4" t="s">
+    <row r="41" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H41" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I41" t="s">
         <v>102</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F26">
-    <sortCondition ref="A3"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:G30">
+    <sortCondition ref="B4"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added FARPs, helos and corrected assets list
</commit_message>
<xml_diff>
--- a/doc/TR_AD_doc_ATO.xlsx
+++ b/doc/TR_AD_doc_ATO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\couby\Saved Games\DCS.openbeta\Missions\735th_Training_AirDefense_Mission\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\735th_Training_AirDefense_Mission\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF64989-47D5-478C-8509-4FF1C4D5014C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6F5031-8DF0-4E07-B943-DAF43D81BEF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blue ATO" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="145">
   <si>
     <t>Task</t>
   </si>
@@ -430,6 +430,39 @@
   </si>
   <si>
     <t>Deep Strike area 1</t>
+  </si>
+  <si>
+    <t>Heavy 1</t>
+  </si>
+  <si>
+    <t>Mi8</t>
+  </si>
+  <si>
+    <t>FARP Moscow</t>
+  </si>
+  <si>
+    <t>Gunship 1</t>
+  </si>
+  <si>
+    <t>UH-1</t>
+  </si>
+  <si>
+    <t>Shark 1</t>
+  </si>
+  <si>
+    <t>Ka-50</t>
+  </si>
+  <si>
+    <t>FARP Warsaw</t>
+  </si>
+  <si>
+    <t>Heavy 2</t>
+  </si>
+  <si>
+    <t>Gunship 2</t>
+  </si>
+  <si>
+    <t>Shark 2</t>
   </si>
 </sst>
 </file>
@@ -667,6 +700,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -685,7 +719,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -972,13 +1005,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>251459</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>151</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1021,13 +1054,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>251459</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>152</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1658,13 +1691,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>208597</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>249799</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2636,7 +2669,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="268605" cy="243762"/>
@@ -2680,7 +2713,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>19047</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>18482</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="219077" cy="240431"/>
@@ -2773,7 +2806,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>57152</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="251999" cy="157161"/>
@@ -2866,7 +2899,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>995363</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>44663</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="290512" cy="169650"/>
@@ -2959,7 +2992,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>66677</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="242168" cy="161923"/>
@@ -3003,7 +3036,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>26670</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="243840" cy="211455"/>
@@ -3047,7 +3080,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="229552" cy="169079"/>
@@ -3087,99 +3120,504 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>73646</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="242887" cy="150191"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="Image 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7611302-FF93-4371-8DC3-822144124A0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="33933" t="23627" r="33894" b="24343"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1203635" y="11162023"/>
+          <a:ext cx="150191" cy="242887"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>73646</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="242887" cy="150191"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Image 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CC76993-4B9A-4EA5-9C3B-3FB83ADEFA25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="33933" t="23627" r="33894" b="24343"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1203635" y="13295623"/>
+          <a:ext cx="150191" cy="242887"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>73646</xdr:rowOff>
     </xdr:from>
+    <xdr:ext cx="242887" cy="150191"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Image 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5941F766-7A28-4C1C-8147-0F7B2721FB98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="33933" t="23627" r="33894" b="24343"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1203635" y="12495523"/>
+          <a:ext cx="150191" cy="242887"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>223837</xdr:rowOff>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>257176</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Image 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C149DF33-2C2D-48D7-9F19-8B9C4B5E0C9F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="33933" t="23627" r="33894" b="24343"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="1203635" y="11162023"/>
-          <a:ext cx="150191" cy="242887"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <xdr:cNvPr id="66" name="Picture 65" descr="Army helicopter bottom view - Free transport icons">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D03EEEC-6403-47C5-8AB9-1973186946B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1162051" y="11449051"/>
+          <a:ext cx="209550" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>73646</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="242887" cy="150191"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="73" name="Image 72">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7611302-FF93-4371-8DC3-822144124A0F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="33933" t="23627" r="33894" b="24343"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="1203635" y="11162023"/>
-          <a:ext cx="150191" cy="242887"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="Picture 74" descr="Army helicopter bottom view - Free transport icons">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E24A8E2D-772D-4730-B628-D3586DE3C692}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1162050" y="12239625"/>
+          <a:ext cx="209550" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="76" name="Picture 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C2C8E56-6055-473C-89CB-835176385FC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1152525" y="11696700"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="77" name="Picture 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC0A23A4-1687-4218-999B-1CC16947513C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1152525" y="11963400"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="78" name="Picture 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EBDDC0B-7EBA-40AA-A330-807E751439C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1162050" y="12496800"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="79" name="Picture 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0006EB31-82EC-4436-ACB9-359F0D623467}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1162050" y="12753975"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5314,13 +5752,13 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="B1:I61"/>
+  <dimension ref="B1:I67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -5338,28 +5776,28 @@
   <sheetData>
     <row r="1" spans="2:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
     </row>
     <row r="3" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="31"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
@@ -5988,16 +6426,16 @@
       <c r="I34" s="23"/>
     </row>
     <row r="35" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="31"/>
     </row>
     <row r="36" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
@@ -6161,18 +6599,18 @@
     </row>
     <row r="44" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="12" t="s">
-        <v>48</v>
+        <v>134</v>
       </c>
       <c r="C44" s="13"/>
       <c r="D44" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="F44" s="15"/>
-      <c r="G44" s="31" t="s">
-        <v>117</v>
+      <c r="G44" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="H44" s="16" t="s">
         <v>85</v>
@@ -6181,18 +6619,17 @@
     </row>
     <row r="45" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C45" s="13"/>
+        <v>137</v>
+      </c>
       <c r="D45" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" s="31" t="s">
-        <v>133</v>
+        <v>138</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="F45" s="15"/>
-      <c r="G45" s="31" t="s">
-        <v>117</v>
+      <c r="G45" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="H45" s="16" t="s">
         <v>85</v>
@@ -6201,18 +6638,18 @@
     </row>
     <row r="46" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
       <c r="C46" s="13"/>
       <c r="D46" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>133</v>
+        <v>140</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="F46" s="15"/>
-      <c r="G46" s="31" t="s">
-        <v>117</v>
+      <c r="G46" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="H46" s="16" t="s">
         <v>85</v>
@@ -6221,38 +6658,38 @@
     </row>
     <row r="47" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E47" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="F47" s="15"/>
-      <c r="G47" s="31" t="s">
-        <v>117</v>
+      <c r="G47" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="H47" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="I47" s="23"/>
+      <c r="I47" s="22"/>
     </row>
     <row r="48" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="12" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E48" s="31" t="s">
-        <v>133</v>
+        <v>138</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="F48" s="15"/>
-      <c r="G48" s="31" t="s">
-        <v>117</v>
+      <c r="G48" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="H48" s="16" t="s">
         <v>85</v>
@@ -6261,18 +6698,18 @@
     </row>
     <row r="49" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="12" t="s">
-        <v>50</v>
+        <v>144</v>
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E49" s="31" t="s">
-        <v>133</v>
+        <v>140</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="F49" s="15"/>
-      <c r="G49" s="31" t="s">
-        <v>117</v>
+      <c r="G49" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="H49" s="16" t="s">
         <v>85</v>
@@ -6281,17 +6718,17 @@
     </row>
     <row r="50" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="E50" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="25" t="s">
         <v>133</v>
       </c>
       <c r="F50" s="15"/>
-      <c r="G50" s="31" t="s">
+      <c r="G50" s="25" t="s">
         <v>117</v>
       </c>
       <c r="H50" s="16" t="s">
@@ -6301,60 +6738,78 @@
     </row>
     <row r="51" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="12" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E51" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="25" t="s">
         <v>133</v>
       </c>
       <c r="F51" s="15"/>
-      <c r="G51" s="31" t="s">
+      <c r="G51" s="25" t="s">
         <v>117</v>
       </c>
       <c r="H51" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="I51" s="23"/>
+      <c r="I51" s="22"/>
     </row>
     <row r="52" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="12"/>
+      <c r="B52" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="C52" s="13"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
+      <c r="D52" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>133</v>
+      </c>
       <c r="F52" s="15"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="23"/>
-    </row>
-    <row r="53" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29"/>
-      <c r="I53" s="30"/>
+      <c r="G52" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I52" s="22"/>
+    </row>
+    <row r="53" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="F53" s="15"/>
+      <c r="G53" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H53" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I53" s="23"/>
     </row>
     <row r="54" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="12" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E54" s="20" t="s">
-        <v>108</v>
+        <v>113</v>
+      </c>
+      <c r="E54" s="25" t="s">
+        <v>133</v>
       </c>
       <c r="F54" s="15"/>
-      <c r="G54" s="20" t="s">
-        <v>77</v>
+      <c r="G54" s="25" t="s">
+        <v>117</v>
       </c>
       <c r="H54" s="16" t="s">
         <v>85</v>
@@ -6363,18 +6818,18 @@
     </row>
     <row r="55" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="12" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E55" s="18" t="s">
-        <v>108</v>
+        <v>114</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>133</v>
       </c>
       <c r="F55" s="15"/>
-      <c r="G55" s="18" t="s">
-        <v>6</v>
+      <c r="G55" s="25" t="s">
+        <v>117</v>
       </c>
       <c r="H55" s="16" t="s">
         <v>85</v>
@@ -6383,61 +6838,163 @@
     </row>
     <row r="56" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="12" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="F56" s="15"/>
+      <c r="G56" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I56" s="22"/>
+    </row>
+    <row r="57" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="13"/>
+      <c r="D57" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="F57" s="15"/>
+      <c r="G57" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H57" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I57" s="23"/>
+    </row>
+    <row r="58" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="12"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="23"/>
+    </row>
+    <row r="59" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="30"/>
+      <c r="I59" s="31"/>
+    </row>
+    <row r="60" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="13"/>
+      <c r="D60" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F60" s="15"/>
+      <c r="G60" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H60" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I60" s="22"/>
+    </row>
+    <row r="61" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" s="13"/>
+      <c r="D61" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" s="15"/>
+      <c r="G61" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I61" s="22"/>
+    </row>
+    <row r="62" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="13"/>
+      <c r="D62" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E56" s="18" t="s">
+      <c r="E62" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="F56" s="15"/>
-      <c r="G56" s="18" t="s">
+      <c r="F62" s="15"/>
+      <c r="G62" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H56" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I56" s="22"/>
-    </row>
-    <row r="59" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="G59" s="8" t="s">
+      <c r="H62" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I62" s="22"/>
+    </row>
+    <row r="65" spans="7:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G65" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H59" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="I59" s="8" t="s">
+      <c r="H65" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I65" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="G60" s="8"/>
-      <c r="H60" s="9" t="s">
+    <row r="66" spans="7:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G66" s="8"/>
+      <c r="H66" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="I60" s="8" t="s">
+      <c r="I66" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H61" s="4" t="s">
+    <row r="67" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H67" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I67" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:G27">
+  <sortState ref="B5:G27">
     <sortCondition ref="B5"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B59:I59"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6457,7 +7014,7 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
@@ -6962,7 +7519,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A44">
+  <sortState ref="A1:A44">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6981,7 +7538,7 @@
       <selection activeCell="B53" sqref="B53:I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -7828,11 +8385,11 @@
       <c r="D44" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E44" s="25" t="s">
         <v>133</v>
       </c>
       <c r="F44" s="15"/>
-      <c r="G44" s="31" t="s">
+      <c r="G44" s="25" t="s">
         <v>117</v>
       </c>
       <c r="H44" s="16" t="s">
@@ -7848,11 +8405,11 @@
       <c r="D45" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E45" s="25" t="s">
         <v>133</v>
       </c>
       <c r="F45" s="15"/>
-      <c r="G45" s="31" t="s">
+      <c r="G45" s="25" t="s">
         <v>117</v>
       </c>
       <c r="H45" s="16" t="s">
@@ -7868,11 +8425,11 @@
       <c r="D46" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="31" t="s">
+      <c r="E46" s="25" t="s">
         <v>133</v>
       </c>
       <c r="F46" s="15"/>
-      <c r="G46" s="31" t="s">
+      <c r="G46" s="25" t="s">
         <v>117</v>
       </c>
       <c r="H46" s="16" t="s">
@@ -7888,11 +8445,11 @@
       <c r="D47" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E47" s="31" t="s">
+      <c r="E47" s="25" t="s">
         <v>133</v>
       </c>
       <c r="F47" s="15"/>
-      <c r="G47" s="31" t="s">
+      <c r="G47" s="25" t="s">
         <v>117</v>
       </c>
       <c r="H47" s="16" t="s">
@@ -7908,11 +8465,11 @@
       <c r="D48" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="E48" s="31" t="s">
+      <c r="E48" s="25" t="s">
         <v>133</v>
       </c>
       <c r="F48" s="15"/>
-      <c r="G48" s="31" t="s">
+      <c r="G48" s="25" t="s">
         <v>117</v>
       </c>
       <c r="H48" s="16" t="s">
@@ -7928,11 +8485,11 @@
       <c r="D49" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E49" s="31" t="s">
+      <c r="E49" s="25" t="s">
         <v>133</v>
       </c>
       <c r="F49" s="15"/>
-      <c r="G49" s="31" t="s">
+      <c r="G49" s="25" t="s">
         <v>117</v>
       </c>
       <c r="H49" s="16" t="s">
@@ -7948,11 +8505,11 @@
       <c r="D50" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="E50" s="31" t="s">
+      <c r="E50" s="25" t="s">
         <v>133</v>
       </c>
       <c r="F50" s="15"/>
-      <c r="G50" s="31" t="s">
+      <c r="G50" s="25" t="s">
         <v>117</v>
       </c>
       <c r="H50" s="16" t="s">
@@ -7968,11 +8525,11 @@
       <c r="D51" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E51" s="31" t="s">
+      <c r="E51" s="25" t="s">
         <v>133</v>
       </c>
       <c r="F51" s="15"/>
-      <c r="G51" s="31" t="s">
+      <c r="G51" s="25" t="s">
         <v>117</v>
       </c>
       <c r="H51" s="16" t="s">
@@ -8113,7 +8670,7 @@
       <selection sqref="A1:B253"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.7109375" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
BFM/ACM training flight added. Resolve #32
</commit_message>
<xml_diff>
--- a/doc/TR_AD_doc_ATO.xlsx
+++ b/doc/TR_AD_doc_ATO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\735th_Training_AirDefense_Mission\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\couby\Saved Games\DCS.openbeta\Missions\735th_Training_AirDefense_Mission\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6F5031-8DF0-4E07-B943-DAF43D81BEF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CE7D6C-85E9-4A6D-B325-F42F5AC6BF27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="2385" windowWidth="27210" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blue ATO" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="150">
   <si>
     <t>Task</t>
   </si>
@@ -463,6 +463,21 @@
   </si>
   <si>
     <t>Shark 2</t>
+  </si>
+  <si>
+    <t>BFM / ACM</t>
+  </si>
+  <si>
+    <t>BFM / ACM #001</t>
+  </si>
+  <si>
+    <t>BFM / ACM #002</t>
+  </si>
+  <si>
+    <t>BFM / ACM #003</t>
+  </si>
+  <si>
+    <t>BFM / ACM #004</t>
   </si>
 </sst>
 </file>
@@ -526,7 +541,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,6 +599,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -737,6 +758,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,13 +1027,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>251459</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>151</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1054,13 +1076,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>251459</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>152</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1691,13 +1713,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>208597</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>249799</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2849,13 +2871,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>995363</xdr:colOff>
+      <xdr:colOff>1033463</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>44663</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>214313</xdr:rowOff>
     </xdr:to>
@@ -2885,7 +2907,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1189144" y="10585557"/>
+          <a:off x="1227244" y="10585557"/>
           <a:ext cx="169650" cy="290512"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2898,7 +2920,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>995363</xdr:colOff>
+      <xdr:colOff>1042988</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>44663</xdr:rowOff>
     </xdr:from>
@@ -2929,7 +2951,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1189144" y="10585557"/>
+          <a:off x="1236769" y="14319357"/>
           <a:ext cx="169650" cy="290512"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3618,6 +3640,226 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="243840" cy="211455"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Image 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6623157-A7CC-4C18-B3D8-D2EA84324397}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22804" t="22479" r="29521" b="23137"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1149667" y="9278303"/>
+          <a:ext cx="211455" cy="243840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="229552" cy="169079"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Image 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CED52ECA-3362-48F5-BC7A-A45F797CE02A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="30889" t="23421" r="30957" b="23605"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1163711" y="9548104"/>
+          <a:ext cx="169079" cy="229552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="268605" cy="243762"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="80" name="Image 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99DD96B9-73AA-4FA1-864E-85A28DDA831D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1145897" y="9815473"/>
+          <a:ext cx="243762" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>17145</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="268605" cy="241857"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="81" name="Image 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB9DD92D-7384-4DAC-B0DD-47BB6F7555B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="26302" t="22986" r="25978" b="24140"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1146849" y="9804996"/>
+          <a:ext cx="241857" cy="268605"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="242887" cy="150191"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="83" name="Image 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BED869FD-6916-491C-8736-F02F24FDE6AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="33933" t="23627" r="33894" b="24343"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1208398" y="16479527"/>
+          <a:ext cx="150191" cy="242887"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5752,16 +5994,16 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="B1:I67"/>
+  <dimension ref="B1:I73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:B46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="4" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
@@ -6888,7 +7130,7 @@
     </row>
     <row r="59" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="29" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
@@ -6900,100 +7142,187 @@
     </row>
     <row r="60" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="12" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="C60" s="13"/>
       <c r="D60" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E60" s="20" t="s">
-        <v>108</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E60" s="38"/>
       <c r="F60" s="15"/>
-      <c r="G60" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H60" s="16" t="s">
-        <v>85</v>
+      <c r="G60" s="38"/>
+      <c r="H60" s="21" t="s">
+        <v>88</v>
       </c>
       <c r="I60" s="22"/>
     </row>
     <row r="61" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="12" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="C61" s="13"/>
       <c r="D61" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E61" s="18" t="s">
-        <v>108</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E61" s="38"/>
       <c r="F61" s="15"/>
-      <c r="G61" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H61" s="16" t="s">
-        <v>85</v>
+      <c r="G61" s="38"/>
+      <c r="H61" s="21" t="s">
+        <v>88</v>
       </c>
       <c r="I61" s="22"/>
     </row>
     <row r="62" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="12" t="s">
-        <v>78</v>
+        <v>148</v>
       </c>
       <c r="C62" s="13"/>
       <c r="D62" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="38"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I62" s="22"/>
+    </row>
+    <row r="63" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E63" s="38"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I63" s="22"/>
+    </row>
+    <row r="64" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="12"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="23"/>
+    </row>
+    <row r="65" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="30"/>
+      <c r="I65" s="31"/>
+    </row>
+    <row r="66" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" s="13"/>
+      <c r="D66" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F66" s="15"/>
+      <c r="G66" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H66" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I66" s="22"/>
+    </row>
+    <row r="67" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" s="13"/>
+      <c r="D67" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E67" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="F67" s="15"/>
+      <c r="G67" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H67" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I67" s="22"/>
+    </row>
+    <row r="68" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68" s="13"/>
+      <c r="D68" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E62" s="18" t="s">
+      <c r="E68" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="F62" s="15"/>
-      <c r="G62" s="18" t="s">
+      <c r="F68" s="15"/>
+      <c r="G68" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H62" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I62" s="22"/>
-    </row>
-    <row r="65" spans="7:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="G65" s="8" t="s">
+      <c r="H68" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I68" s="22"/>
+    </row>
+    <row r="71" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G71" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H65" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="I65" s="8" t="s">
+      <c r="H71" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I71" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="7:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="G66" s="8"/>
-      <c r="H66" s="9" t="s">
+    <row r="72" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G72" s="8"/>
+      <c r="H72" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="I66" s="8" t="s">
+      <c r="I72" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H67" s="4" t="s">
+    <row r="73" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H73" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I73" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B5:G27">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:G27">
     <sortCondition ref="B5"/>
   </sortState>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B65:I65"/>
     <mergeCell ref="B59:I59"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7014,7 +7343,7 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
@@ -7519,7 +7848,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A44">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A44">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7538,7 +7867,7 @@
       <selection activeCell="B53" sqref="B53:I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -8670,7 +8999,7 @@
       <selection sqref="A1:B253"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.7109375" customWidth="1"/>
   </cols>

</xml_diff>